<commit_message>
Modificação do arquivo teste.
</commit_message>
<xml_diff>
--- a/diabetesTeste.xlsx
+++ b/diabetesTeste.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="10" documentId="11_AD4D361C20488DEA4E38A04D2C1D771E5BDEDD8F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64E349D8-6032-4A4F-AAE0-888EFEB4580C}"/>
   <bookViews>
-    <workbookView xWindow="3705" yWindow="6465" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -140,6 +140,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>